<commit_message>
Updated visualization for improved results
</commit_message>
<xml_diff>
--- a/Q1 - Rxn_Analysis.xlsx
+++ b/Q1 - Rxn_Analysis.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding Related Items\Web Dev\python\plots for dr reddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65BB278-5D1E-4F1B-B910-0715F480F90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F8E87E-2658-452A-A87C-BD9E0C4FCEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Condition_by_Condition" sheetId="1" r:id="rId1"/>
     <sheet name="Overall_Rankings" sheetId="2" r:id="rId2"/>
+    <sheet name="Kinetic_Formulas_and_Methods" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
   <si>
     <t>reaction</t>
   </si>
@@ -32,9 +33,6 @@
     <t>concentration</t>
   </si>
   <si>
-    <t>selectivity</t>
-  </si>
-  <si>
     <t>temp_sensitivity</t>
   </si>
   <si>
@@ -44,6 +42,12 @@
     <t>rate_constant</t>
   </si>
   <si>
+    <t>kinetic_model</t>
+  </si>
+  <si>
+    <t>r_squared</t>
+  </si>
+  <si>
     <t>impurity_formation</t>
   </si>
   <si>
@@ -74,6 +78,9 @@
     <t>R1</t>
   </si>
   <si>
+    <t>first_order</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
@@ -89,9 +96,6 @@
     <t>first_place_count</t>
   </si>
   <si>
-    <t>avg_selectivity</t>
-  </si>
-  <si>
     <t>avg_yield</t>
   </si>
   <si>
@@ -110,7 +114,151 @@
     <t>avg_conc_sensitivity</t>
   </si>
   <si>
+    <t>avg_r_squared</t>
+  </si>
+  <si>
     <t>conditions_analyzed</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Formula/Description</t>
+  </si>
+  <si>
+    <t>KINETIC ANALYSIS FORMULAS</t>
+  </si>
+  <si>
+    <t>Zero-order reaction:</t>
+  </si>
+  <si>
+    <t>[A] = [A₀] - kt</t>
+  </si>
+  <si>
+    <t>Zero-order rate constant:</t>
+  </si>
+  <si>
+    <t>k = (A₀ - A) / t</t>
+  </si>
+  <si>
+    <t>Zero-order units:</t>
+  </si>
+  <si>
+    <t>mg/mL/h</t>
+  </si>
+  <si>
+    <t>First-order reaction:</t>
+  </si>
+  <si>
+    <t>[A] = [A₀] * exp(-kt)</t>
+  </si>
+  <si>
+    <t>First-order rate constant:</t>
+  </si>
+  <si>
+    <t>k = -ln([A]/[A₀]) / t</t>
+  </si>
+  <si>
+    <t>First-order units:</t>
+  </si>
+  <si>
+    <t>1/h</t>
+  </si>
+  <si>
+    <t>Second-order reaction:</t>
+  </si>
+  <si>
+    <t>1/[A] = 1/[A₀] + kt</t>
+  </si>
+  <si>
+    <t>Second-order rate constant:</t>
+  </si>
+  <si>
+    <t>k = (1/[A] - 1/[A₀]) / t</t>
+  </si>
+  <si>
+    <t>Second-order units:</t>
+  </si>
+  <si>
+    <t>mL/mg/h</t>
+  </si>
+  <si>
+    <t>R² (Coefficient of Determination):</t>
+  </si>
+  <si>
+    <t>R² = 1 - (SS_res / SS_tot)</t>
+  </si>
+  <si>
+    <t>R² interpretation:</t>
+  </si>
+  <si>
+    <t>R² &gt; 0.95 = excellent fit</t>
+  </si>
+  <si>
+    <t>R² &gt; 0.90 = good fit</t>
+  </si>
+  <si>
+    <t>R² &gt; 0.80 = acceptable fit</t>
+  </si>
+  <si>
+    <t>Best Model Selection:</t>
+  </si>
+  <si>
+    <t>Highest R² value determines best kinetic model</t>
+  </si>
+  <si>
+    <t>RANKING METHODOLOGY</t>
+  </si>
+  <si>
+    <t>Priority 1 (Weight: 1.0):</t>
+  </si>
+  <si>
+    <t>Impurity Formation (minimize)</t>
+  </si>
+  <si>
+    <t>Priority 2 (Weight: 0.9):</t>
+  </si>
+  <si>
+    <t>Yield (maximize)</t>
+  </si>
+  <si>
+    <t>Priority 3 (Weight: 0.85):</t>
+  </si>
+  <si>
+    <t>Conversion (maximize)</t>
+  </si>
+  <si>
+    <t>Priority 4 (Weight: 0.55):</t>
+  </si>
+  <si>
+    <t>Rate Constant (maximize)</t>
+  </si>
+  <si>
+    <t>Priority 5 (Weight: 0.4):</t>
+  </si>
+  <si>
+    <t>Temperature Sensitivity (minimize)</t>
+  </si>
+  <si>
+    <t>Concentration Sensitivity (minimize)</t>
+  </si>
+  <si>
+    <t>Final Score:</t>
+  </si>
+  <si>
+    <t>Weighted sum of normalized metrics</t>
+  </si>
+  <si>
+    <t>Normalization:</t>
+  </si>
+  <si>
+    <t>All metrics scaled to 0-1 range</t>
+  </si>
+  <si>
+    <t>Ranking:</t>
+  </si>
+  <si>
+    <t>Highest score = best reaction</t>
   </si>
 </sst>
 </file>
@@ -473,25 +621,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" customWidth="1"/>
-    <col min="11" max="11" width="20.5546875" customWidth="1"/>
-    <col min="15" max="15" width="23.44140625" customWidth="1"/>
-    <col min="16" max="16" width="20.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,10 +681,13 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>30</v>
@@ -552,48 +696,51 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <v>98.727970580551826</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E2">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F2">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G2">
-        <v>19.905200000000001</v>
+        <v>1.0797013625471099</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
       </c>
       <c r="H2">
+        <v>0.99999374845066535</v>
+      </c>
+      <c r="I2">
         <v>1.266</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>99.525999999999996</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>98.26</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>5</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.23699999999999999</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>49.13</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.63300000000000001</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>30</v>
@@ -602,48 +749,51 @@
         <v>50</v>
       </c>
       <c r="D3">
-        <v>80.643216080401999</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E3">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F3">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G3">
-        <v>2.842857142857143</v>
+        <v>0.1513775166244325</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
       <c r="H3">
+        <v>0.99999999994145605</v>
+      </c>
+      <c r="I3">
         <v>19.262</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>99.5</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>80.239999999999995</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>35</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.25</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>40.119999999999997</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>9.6310000000000002</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2</v>
       </c>
-      <c r="P3">
-        <v>3.3715533690894599</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <v>2.856734072434612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -652,48 +802,51 @@
         <v>50</v>
       </c>
       <c r="D4">
-        <v>30.18089623116084</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E4">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F4">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G4">
-        <v>9.9394000000000009</v>
+        <v>0.51075816231500837</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
       </c>
       <c r="H4">
+        <v>0.99999999962546637</v>
+      </c>
+      <c r="I4">
         <v>69.396000000000001</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>99.394000000000005</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>29.998000000000001</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>10</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.30299999999999999</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>14.999000000000001</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>34.698</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>3</v>
       </c>
-      <c r="P4">
-        <v>0.62416297126593767</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <v>0.6082764822358091</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -702,48 +855,51 @@
         <v>100</v>
       </c>
       <c r="D5">
-        <v>97.498442805762636</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E5">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F5">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G5">
-        <v>19.907599999999999</v>
+        <v>1.0940816306653649</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
       </c>
       <c r="H5">
+        <v>0.99997588114614167</v>
+      </c>
+      <c r="I5">
         <v>2.4889999999999999</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>99.537999999999997</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>97.048000000000002</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>5</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.46200000000000002</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>97.048000000000002</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>2.4889999999999999</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="P5">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>30</v>
@@ -752,48 +908,51 @@
         <v>100</v>
       </c>
       <c r="D6">
-        <v>80.642211055276391</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E6">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F6">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G6">
-        <v>2.842857142857143</v>
+        <v>0.15138033473750681</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
       </c>
       <c r="H6">
+        <v>0.999999999972362</v>
+      </c>
+      <c r="I6">
         <v>19.260999999999999</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>99.5</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>80.239000000000004</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>35</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0.5</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>80.239000000000004</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>19.260999999999999</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>2</v>
       </c>
-      <c r="P6">
-        <v>3.347926146658295</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>2.8237070327764529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -802,48 +961,51 @@
         <v>100</v>
       </c>
       <c r="D7">
-        <v>30.181598671965389</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E7">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F7">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G7">
-        <v>9.9394999999999989</v>
+        <v>0.51076075374751417</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
       </c>
       <c r="H7">
+        <v>0.99999999986355192</v>
+      </c>
+      <c r="I7">
         <v>69.396000000000001</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>99.394999999999996</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>29.998999999999999</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>10</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.60499999999999998</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>29.998999999999999</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>69.396000000000001</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>3</v>
       </c>
-      <c r="P7">
-        <v>0.62413402196784185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <v>0.60502902592763608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -852,48 +1014,51 @@
         <v>200</v>
       </c>
       <c r="D8">
-        <v>95.157167322053652</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E8">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F8">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G8">
-        <v>19.911899999999999</v>
+        <v>1.1226308617040239</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
       </c>
       <c r="H8">
+        <v>0.9999100792657174</v>
+      </c>
+      <c r="I8">
         <v>4.8215000000000003</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>99.5595</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>94.738</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>5</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>0.88100000000000001</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>189.476</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>9.6430000000000007</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>1</v>
       </c>
-      <c r="P8">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>30</v>
@@ -902,48 +1067,51 @@
         <v>200</v>
       </c>
       <c r="D9">
-        <v>80.642211055276391</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E9">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F9">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G9">
-        <v>2.842857142857143</v>
+        <v>0.1513801010764205</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
       </c>
       <c r="H9">
+        <v>0.99999999998870126</v>
+      </c>
+      <c r="I9">
         <v>19.260999999999999</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>99.5</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>80.239000000000004</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>35</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>160.47800000000001</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>38.521999999999998</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>2</v>
       </c>
-      <c r="P9">
-        <v>3.336389906470643</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q9">
+        <v>2.793263504675557</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -952,48 +1120,51 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>30.181598671965389</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E10">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F10">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G10">
-        <v>9.9394999999999989</v>
+        <v>0.51076103422462971</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
       </c>
       <c r="H10">
+        <v>0.99999999997812272</v>
+      </c>
+      <c r="I10">
         <v>69.396000000000001</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>99.394999999999996</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>29.998999999999999</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>10</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1.21</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>59.997999999999998</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>138.792</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>3</v>
       </c>
-      <c r="P10">
-        <v>0.62407640171263845</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q10">
+        <v>0.59886606977792678</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>40</v>
@@ -1002,48 +1173,51 @@
         <v>50</v>
       </c>
       <c r="D11">
-        <v>98.439943854020456</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E11">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F11">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G11">
-        <v>19.948</v>
+        <v>1.2042672894424979</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
       </c>
       <c r="H11">
+        <v>0.99999145643103682</v>
+      </c>
+      <c r="I11">
         <v>1.556</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>99.74</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>98.183999999999997</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>5</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.13</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>49.091999999999999</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.77800000000000002</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>1</v>
       </c>
-      <c r="P11">
-        <v>3.7020325203251949</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q11">
+        <v>3.0020325203251961</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>40</v>
@@ -1052,48 +1226,51 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <v>78.703257904028249</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E12">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F12">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G12">
-        <v>2.8484571428571428</v>
+        <v>0.16557236457556329</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
       </c>
       <c r="H12">
+        <v>0.99999999987709587</v>
+      </c>
+      <c r="I12">
         <v>21.231999999999999</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>99.695999999999998</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>78.463999999999999</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>35</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.152</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>39.231999999999999</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>10.616</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>2</v>
       </c>
-      <c r="P12">
-        <v>2.758747493241533</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q12">
+        <v>2.2253030382020871</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>40</v>
@@ -1102,48 +1279,51 @@
         <v>50</v>
       </c>
       <c r="D13">
-        <v>15.24083968701847</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E13">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F13">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G13">
-        <v>9.9941999999999993</v>
+        <v>0.74430305697829957</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
       </c>
       <c r="H13">
+        <v>0.99999999956923302</v>
+      </c>
+      <c r="I13">
         <v>84.707999999999998</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>99.941999999999993</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>15.231999999999999</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>10</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>7.6159999999999997</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>42.353999999999999</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>3</v>
       </c>
-      <c r="P13">
-        <v>1.475247813654563</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q13">
+        <v>1.5517998421032211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>40</v>
@@ -1152,48 +1332,51 @@
         <v>100</v>
       </c>
       <c r="D14">
-        <v>96.9422945823475</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E14">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F14">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G14">
-        <v>19.9496</v>
+        <v>1.224069056636742</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
       </c>
       <c r="H14">
+        <v>0.99996740263301032</v>
+      </c>
+      <c r="I14">
         <v>3.05</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>99.748000000000005</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>96.697999999999993</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>5</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.252</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>96.697999999999993</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>3.05</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>1</v>
       </c>
-      <c r="P14">
-        <v>3.7304081632653259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <v>3.0304081632653261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>40</v>
@@ -1202,48 +1385,51 @@
         <v>100</v>
       </c>
       <c r="D15">
-        <v>78.703257904028249</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E15">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F15">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G15">
-        <v>2.8484571428571428</v>
+        <v>0.16557385736778019</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
       </c>
       <c r="H15">
+        <v>0.99999999994437139</v>
+      </c>
+      <c r="I15">
         <v>21.231999999999999</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>99.695999999999998</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>78.463999999999999</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>35</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>0.30399999999999999</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>78.463999999999999</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>21.231999999999999</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>2</v>
       </c>
-      <c r="P15">
-        <v>2.7950136470316811</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q15">
+        <v>2.251783794715152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>40</v>
@@ -1252,48 +1438,51 @@
         <v>100</v>
       </c>
       <c r="D16">
-        <v>15.241992775737691</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E16">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F16">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G16">
-        <v>9.9940999999999995</v>
+        <v>0.74431055138421798</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
       </c>
       <c r="H16">
+        <v>0.99999999984169019</v>
+      </c>
+      <c r="I16">
         <v>84.709000000000003</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>99.941000000000003</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>15.233000000000001</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>10</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>15.233000000000001</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>84.709000000000003</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>3</v>
       </c>
-      <c r="P16">
-        <v>1.4752230934373269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16">
+        <v>1.546070599853572</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>40</v>
@@ -1302,48 +1491,51 @@
         <v>200</v>
       </c>
       <c r="D17">
-        <v>94.12003508332289</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E17">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F17">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G17">
-        <v>19.952500000000001</v>
+        <v>1.263374602606619</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
       </c>
       <c r="H17">
+        <v>0.99988106650138076</v>
+      </c>
+      <c r="I17">
         <v>5.8659999999999997</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>99.762500000000003</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>93.896500000000003</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>5</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>0.47499999999999998</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>187.79300000000001</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>11.731999999999999</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>1</v>
       </c>
-      <c r="P17">
-        <v>3.7815040650406671</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q17">
+        <v>3.081504065040666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -1352,48 +1544,51 @@
         <v>200</v>
       </c>
       <c r="D18">
-        <v>78.703652622234713</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E18">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F18">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G18">
-        <v>2.8484428571428571</v>
+        <v>0.16557156501635101</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
       </c>
       <c r="H18">
+        <v>0.99999999998624634</v>
+      </c>
+      <c r="I18">
         <v>21.231999999999999</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>99.695499999999996</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>78.463999999999999</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>35</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>0.60899999999999999</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>156.928</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>42.463999999999999</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>2</v>
       </c>
-      <c r="P18">
-        <v>2.8671161271022489</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q18">
+        <v>2.3044270993386551</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>40</v>
@@ -1402,48 +1597,51 @@
         <v>200</v>
       </c>
       <c r="D19">
-        <v>15.241416228493669</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E19">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F19">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G19">
-        <v>9.9941500000000012</v>
+        <v>0.74430691846032937</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
       </c>
       <c r="H19">
+        <v>0.99999999996722555</v>
+      </c>
+      <c r="I19">
         <v>84.709000000000003</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>99.941500000000005</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>15.2325</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>10</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>0.11700000000000001</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>30.465</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>169.41800000000001</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>3</v>
       </c>
-      <c r="P19">
-        <v>1.475186003396205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q19">
+        <v>1.535302560410871</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -1452,48 +1650,51 @@
         <v>50</v>
       </c>
       <c r="D20">
-        <v>98.143735357135711</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E20">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F20">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G20">
-        <v>19.9756</v>
+        <v>1.3603632726684449</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
       </c>
       <c r="H20">
+        <v>0.99998938914557312</v>
+      </c>
+      <c r="I20">
         <v>1.8540000000000001</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>99.878</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>98.024000000000001</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>5</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>49.012</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>0.92700000000000005</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>1</v>
       </c>
-      <c r="P20">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q20">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>50</v>
@@ -1502,48 +1703,51 @@
         <v>50</v>
       </c>
       <c r="D21">
-        <v>77.219071286850919</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E21">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F21">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G21">
-        <v>2.8512571428571429</v>
+        <v>0.17660896047842531</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
       </c>
       <c r="H21">
+        <v>0.99999999982816123</v>
+      </c>
+      <c r="I21">
         <v>22.734000000000002</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>99.793999999999997</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>77.06</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>35</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>0.10299999999999999</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>38.53</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>11.367000000000001</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>2</v>
       </c>
-      <c r="P21">
-        <v>2.7851517438971221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q21">
+        <v>2.2445163575111988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>50</v>
@@ -1552,48 +1756,51 @@
         <v>50</v>
       </c>
       <c r="D22">
-        <v>5.944118882377647</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E22">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F22">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G22">
-        <v>9.9998000000000005</v>
+        <v>1.059661002101669</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
       </c>
       <c r="H22">
+        <v>0.99999999939626516</v>
+      </c>
+      <c r="I22">
         <v>94.054000000000002</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>99.998000000000005</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>5.944</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>10</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>1E-3</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>2.972</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>47.027000000000001</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>3</v>
       </c>
-      <c r="P22">
-        <v>1.475004882786253</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q22">
+        <v>1.655642467619151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>50</v>
@@ -1602,48 +1809,51 @@
         <v>100</v>
       </c>
       <c r="D23">
-        <v>96.376724534951236</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E23">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F23">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G23">
-        <v>19.976400000000002</v>
+        <v>1.387064749020035</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
       </c>
       <c r="H23">
+        <v>0.99996006278525629</v>
+      </c>
+      <c r="I23">
         <v>3.6190000000000002</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>99.882000000000005</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>96.263000000000005</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>5</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>0.11799999999999999</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>96.263000000000005</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>3.6190000000000002</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>1</v>
       </c>
-      <c r="P23">
-        <v>3.9208333333333392</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q23">
+        <v>3.220833333333339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>50</v>
@@ -1652,48 +1862,51 @@
         <v>100</v>
       </c>
       <c r="D24">
-        <v>77.218843005020389</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E24">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F24">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G24">
-        <v>2.851228571428571</v>
+        <v>0.1766107111994524</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
       </c>
       <c r="H24">
+        <v>0.99999999996429145</v>
+      </c>
+      <c r="I24">
         <v>22.734000000000002</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>99.793000000000006</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>77.058999999999997</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>35</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>0.20699999999999999</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>77.058999999999997</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>22.734000000000002</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>2</v>
       </c>
-      <c r="P24">
-        <v>2.8243667983695961</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q24">
+        <v>2.2731581060420818</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>50</v>
@@ -1702,48 +1915,51 @@
         <v>100</v>
       </c>
       <c r="D25">
-        <v>5.9431782953488614</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E25">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F25">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G25">
-        <v>9.9997000000000007</v>
+        <v>1.059666455682426</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
       </c>
       <c r="H25">
+        <v>0.99999999988894084</v>
+      </c>
+      <c r="I25">
         <v>94.054000000000002</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>99.997</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>5.9429999999999996</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>10</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>5.9429999999999996</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>94.054000000000002</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>3</v>
       </c>
-      <c r="P25">
-        <v>1.4749914801018229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q25">
+        <v>1.646594205739478</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26">
         <v>50</v>
@@ -1752,48 +1968,51 @@
         <v>200</v>
       </c>
       <c r="D26">
-        <v>93.080353790939</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E26">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F26">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G26">
-        <v>19.977900000000002</v>
+        <v>1.440003095195352</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
       </c>
       <c r="H26">
+        <v>0.99985769829773641</v>
+      </c>
+      <c r="I26">
         <v>6.9124999999999996</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>99.889499999999998</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>92.977500000000006</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>5</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>0.221</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>185.95500000000001</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>13.824999999999999</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>1</v>
       </c>
-      <c r="P26">
-        <v>3.9511002444987509</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q26">
+        <v>3.251100244498752</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B27">
         <v>50</v>
@@ -1802,48 +2021,51 @@
         <v>200</v>
       </c>
       <c r="D27">
-        <v>77.219344042167279</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E27">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F27">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G27">
-        <v>2.851228571428571</v>
+        <v>0.17660998221301599</v>
+      </c>
+      <c r="G27" t="s">
+        <v>18</v>
       </c>
       <c r="H27">
+        <v>0.99999999998712019</v>
+      </c>
+      <c r="I27">
         <v>22.734000000000002</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>99.793000000000006</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>77.0595</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>35</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>0.41399999999999998</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>154.119</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>45.468000000000004</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>2</v>
       </c>
-      <c r="P27">
-        <v>2.901803361749447</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q27">
+        <v>2.3297203768583761</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B28">
         <v>50</v>
@@ -1852,48 +2074,51 @@
         <v>200</v>
       </c>
       <c r="D28">
-        <v>5.9436485912147807</v>
+        <v>1.0328250276619559</v>
       </c>
       <c r="E28">
-        <v>1.035214093657288</v>
+        <v>2.1132402255538891E-4</v>
       </c>
       <c r="F28">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G28">
-        <v>9.9997500000000006</v>
+        <v>1.059657872101226</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
       </c>
       <c r="H28">
+        <v>0.9999999999613558</v>
+      </c>
+      <c r="I28">
         <v>94.054500000000004</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>99.997500000000002</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>5.9435000000000002</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>10</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>11.887</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>188.10900000000001</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>3</v>
       </c>
-      <c r="P28">
-        <v>1.474972978230662</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q28">
+        <v>1.6297779745807781</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <v>60</v>
@@ -1902,48 +2127,51 @@
         <v>50</v>
       </c>
       <c r="D29">
-        <v>98.337933517340701</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E29">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F29">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G29">
-        <v>19.999199999999998</v>
+        <v>2.017297992778738</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
       </c>
       <c r="H29">
+        <v>0.99999556393561462</v>
+      </c>
+      <c r="I29">
         <v>1.6619999999999999</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>99.995999999999995</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>98.334000000000003</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>5</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>2E-3</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>49.167000000000002</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>0.83099999999999996</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>1</v>
       </c>
-      <c r="P29">
-        <v>4.3433333333332662</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q29">
+        <v>3.643333333333266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B30">
         <v>60</v>
@@ -1952,48 +2180,51 @@
         <v>50</v>
       </c>
       <c r="D30">
-        <v>72.62557534520711</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E30">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F30">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G30">
-        <v>2.855428571428571</v>
+        <v>0.21192891652477461</v>
+      </c>
+      <c r="G30" t="s">
+        <v>18</v>
       </c>
       <c r="H30">
+        <v>0.99999999982480225</v>
+      </c>
+      <c r="I30">
         <v>27.358000000000001</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>99.94</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>72.581999999999994</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>35</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>0.03</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>36.290999999999997</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>13.679</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>2</v>
       </c>
-      <c r="P30">
-        <v>2.683396196626719</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q30">
+        <v>2.1701444043267428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B31">
         <v>60</v>
@@ -2002,48 +2233,51 @@
         <v>50</v>
       </c>
       <c r="D31">
+        <v>1.0328250276619559</v>
+      </c>
+      <c r="E31">
+        <v>2.1132402255538891E-4</v>
+      </c>
+      <c r="F31">
+        <v>1.476977430701629</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31">
+        <v>0.99999999959387198</v>
+      </c>
+      <c r="I31">
+        <v>98.3</v>
+      </c>
+      <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31">
         <v>1.7</v>
       </c>
-      <c r="E31">
-        <v>1.035214093657288</v>
-      </c>
-      <c r="F31">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G31">
+      <c r="L31">
         <v>10</v>
       </c>
-      <c r="H31">
-        <v>98.3</v>
-      </c>
-      <c r="I31">
-        <v>100</v>
-      </c>
-      <c r="J31">
-        <v>1.7</v>
-      </c>
-      <c r="K31">
-        <v>10</v>
-      </c>
-      <c r="L31">
+      <c r="M31">
         <v>0</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>0.85</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>49.15</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>3</v>
       </c>
-      <c r="P31">
-        <v>1.4746172768040069</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q31">
+        <v>1.630748834243847</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B32">
         <v>60</v>
@@ -2052,48 +2286,51 @@
         <v>100</v>
       </c>
       <c r="D32">
-        <v>96.746837341867092</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E32">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F32">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G32">
-        <v>19.998999999999999</v>
+        <v>2.0523431755517199</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
       </c>
       <c r="H32">
+        <v>0.99998359957776439</v>
+      </c>
+      <c r="I32">
         <v>3.2530000000000001</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>99.995000000000005</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>96.742000000000004</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>5</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>96.742000000000004</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>3.2530000000000001</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>1</v>
       </c>
-      <c r="P32">
-        <v>4.3291666666667341</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q32">
+        <v>3.629166666666733</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B33">
         <v>60</v>
@@ -2102,48 +2339,51 @@
         <v>100</v>
       </c>
       <c r="D33">
-        <v>72.62557534520711</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E33">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F33">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G33">
-        <v>2.855428571428571</v>
+        <v>0.21193394294077339</v>
+      </c>
+      <c r="G33" t="s">
+        <v>18</v>
       </c>
       <c r="H33">
+        <v>0.99999999997523403</v>
+      </c>
+      <c r="I33">
         <v>27.358000000000001</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>99.94</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>72.581999999999994</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>35</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>0.06</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>72.581999999999994</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>27.358000000000001</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>2</v>
       </c>
-      <c r="P33">
-        <v>2.7153383461369391</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q33">
+        <v>2.193488153934092</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B34">
         <v>60</v>
@@ -2152,48 +2392,51 @@
         <v>100</v>
       </c>
       <c r="D34">
+        <v>1.0328250276619559</v>
+      </c>
+      <c r="E34">
+        <v>2.1132402255538891E-4</v>
+      </c>
+      <c r="F34">
+        <v>1.4769727060293509</v>
+      </c>
+      <c r="G34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34">
+        <v>0.99999999989169219</v>
+      </c>
+      <c r="I34">
+        <v>98.3</v>
+      </c>
+      <c r="J34">
+        <v>100</v>
+      </c>
+      <c r="K34">
         <v>1.7010000000000001</v>
       </c>
-      <c r="E34">
-        <v>1.035214093657288</v>
-      </c>
-      <c r="F34">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G34">
+      <c r="L34">
         <v>10</v>
       </c>
-      <c r="H34">
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="O34">
         <v>98.3</v>
       </c>
-      <c r="I34">
-        <v>100</v>
-      </c>
-      <c r="J34">
-        <v>1.7010000000000001</v>
-      </c>
-      <c r="K34">
-        <v>10</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <v>1.7010000000000001</v>
-      </c>
-      <c r="N34">
-        <v>98.3</v>
-      </c>
-      <c r="O34">
+      <c r="P34">
         <v>3</v>
       </c>
-      <c r="P34">
-        <v>1.4746199508027491</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q34">
+        <v>1.623408295324803</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <v>60</v>
@@ -2202,48 +2445,51 @@
         <v>200</v>
       </c>
       <c r="D35">
-        <v>93.757219074858369</v>
+        <v>5.3069273602759067E-3</v>
       </c>
       <c r="E35">
-        <v>5.4209688095402048E-3</v>
+        <v>1.7955562058679719E-2</v>
       </c>
       <c r="F35">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G35">
-        <v>19.999099999999999</v>
+        <v>2.1212999718568568</v>
+      </c>
+      <c r="G35" t="s">
+        <v>18</v>
       </c>
       <c r="H35">
+        <v>0.99994284303413328</v>
+      </c>
+      <c r="I35">
         <v>6.2424999999999997</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>99.995500000000007</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>93.753</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>5</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>187.506</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>12.484999999999999</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>1</v>
       </c>
-      <c r="P35">
-        <v>4.336250000000101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q35">
+        <v>3.6362500000000999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B36">
         <v>60</v>
@@ -2252,48 +2498,51 @@
         <v>200</v>
       </c>
       <c r="D36">
-        <v>72.625075045027017</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E36">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F36">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G36">
-        <v>2.855428571428571</v>
+        <v>0.21193136007736921</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
       </c>
       <c r="H36">
+        <v>0.9999999999814535</v>
+      </c>
+      <c r="I36">
         <v>27.358499999999999</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>99.94</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>72.581500000000005</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>35</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>0.12</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>145.16300000000001</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>54.716999999999999</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>2</v>
       </c>
-      <c r="P36">
-        <v>2.7783221003523022</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q36">
+        <v>2.2395109949815479</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B37">
         <v>60</v>
@@ -2302,48 +2551,51 @@
         <v>200</v>
       </c>
       <c r="D37">
+        <v>1.0328250276619559</v>
+      </c>
+      <c r="E37">
+        <v>2.1132402255538891E-4</v>
+      </c>
+      <c r="F37">
+        <v>1.476968346013356</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37">
+        <v>0.99999999995379329</v>
+      </c>
+      <c r="I37">
+        <v>98.299499999999995</v>
+      </c>
+      <c r="J37">
+        <v>100</v>
+      </c>
+      <c r="K37">
         <v>1.7004999999999999</v>
       </c>
-      <c r="E37">
-        <v>1.035214093657288</v>
-      </c>
-      <c r="F37">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G37">
+      <c r="L37">
         <v>10</v>
       </c>
-      <c r="H37">
-        <v>98.299499999999995</v>
-      </c>
-      <c r="I37">
-        <v>100</v>
-      </c>
-      <c r="J37">
-        <v>1.7004999999999999</v>
-      </c>
-      <c r="K37">
-        <v>10</v>
-      </c>
-      <c r="L37">
+      <c r="M37">
         <v>0</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>3.4009999999999998</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>196.59899999999999</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>3</v>
       </c>
-      <c r="P37">
-        <v>1.474618613795579</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q37">
+        <v>1.609753915925922</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>70</v>
@@ -2352,48 +2604,51 @@
         <v>50</v>
       </c>
       <c r="D38">
+        <v>5.3069273602759067E-3</v>
+      </c>
+      <c r="E38">
+        <v>1.7955562058679719E-2</v>
+      </c>
+      <c r="F38">
+        <v>3.635748448508147</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38">
+        <v>0.99999972934293646</v>
+      </c>
+      <c r="I38">
+        <v>1.216</v>
+      </c>
+      <c r="J38">
+        <v>100</v>
+      </c>
+      <c r="K38">
         <v>98.784000000000006</v>
       </c>
-      <c r="E38">
-        <v>5.4209688095402048E-3</v>
-      </c>
-      <c r="F38">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G38">
-        <v>20</v>
-      </c>
-      <c r="H38">
-        <v>1.216</v>
-      </c>
-      <c r="I38">
-        <v>100</v>
-      </c>
-      <c r="J38">
-        <v>98.784000000000006</v>
-      </c>
-      <c r="K38">
+      <c r="L38">
         <v>5</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>0</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>49.392000000000003</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>0.60799999999999998</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>1</v>
       </c>
-      <c r="P38">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q38">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B39">
         <v>70</v>
@@ -2402,48 +2657,51 @@
         <v>50</v>
       </c>
       <c r="D39">
-        <v>66.208620862086207</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E39">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F39">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G39">
-        <v>2.8568571428571432</v>
+        <v>0.26491250959334939</v>
+      </c>
+      <c r="G39" t="s">
+        <v>18</v>
       </c>
       <c r="H39">
+        <v>0.9999999997246074</v>
+      </c>
+      <c r="I39">
         <v>33.787999999999997</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>99.99</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>66.201999999999998</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>35</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>33.100999999999999</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>16.893999999999998</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <v>2</v>
       </c>
-      <c r="P39">
-        <v>2.51506446418664</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q39">
+        <v>2.047182101813283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B40">
         <v>70</v>
@@ -2452,48 +2710,51 @@
         <v>50</v>
       </c>
       <c r="D40">
+        <v>1.0328250276619559</v>
+      </c>
+      <c r="E40">
+        <v>2.1132402255538891E-4</v>
+      </c>
+      <c r="F40">
+        <v>2.019152651385117</v>
+      </c>
+      <c r="G40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40">
+        <v>0.99999999959114538</v>
+      </c>
+      <c r="I40">
+        <v>99.665999999999997</v>
+      </c>
+      <c r="J40">
+        <v>100</v>
+      </c>
+      <c r="K40">
         <v>0.33400000000000002</v>
       </c>
-      <c r="E40">
-        <v>1.035214093657288</v>
-      </c>
-      <c r="F40">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G40">
+      <c r="L40">
         <v>10</v>
       </c>
-      <c r="H40">
-        <v>99.665999999999997</v>
-      </c>
-      <c r="I40">
-        <v>100</v>
-      </c>
-      <c r="J40">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="K40">
-        <v>10</v>
-      </c>
-      <c r="L40">
+      <c r="M40">
         <v>0</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>0.16700000000000001</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>49.832999999999998</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <v>3</v>
       </c>
-      <c r="P40">
-        <v>1.474579848440692</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q40">
+        <v>1.5315851106316041</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <v>70</v>
@@ -2502,48 +2763,51 @@
         <v>100</v>
       </c>
       <c r="D41">
+        <v>5.3069273602759067E-3</v>
+      </c>
+      <c r="E41">
+        <v>1.7955562058679719E-2</v>
+      </c>
+      <c r="F41">
+        <v>3.67491532759108</v>
+      </c>
+      <c r="G41" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41">
+        <v>0.99999901795994128</v>
+      </c>
+      <c r="I41">
+        <v>2.3959999999999999</v>
+      </c>
+      <c r="J41">
+        <v>100</v>
+      </c>
+      <c r="K41">
         <v>97.603999999999999</v>
       </c>
-      <c r="E41">
-        <v>5.4209688095402048E-3</v>
-      </c>
-      <c r="F41">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G41">
-        <v>20</v>
-      </c>
-      <c r="H41">
+      <c r="L41">
+        <v>5</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>97.603999999999999</v>
+      </c>
+      <c r="O41">
         <v>2.3959999999999999</v>
       </c>
-      <c r="I41">
-        <v>100</v>
-      </c>
-      <c r="J41">
-        <v>97.603999999999999</v>
-      </c>
-      <c r="K41">
-        <v>5</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>97.603999999999999</v>
-      </c>
-      <c r="N41">
-        <v>2.3959999999999999</v>
-      </c>
-      <c r="O41">
+      <c r="P41">
         <v>1</v>
       </c>
-      <c r="P41">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q41">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B42">
         <v>70</v>
@@ -2552,48 +2816,51 @@
         <v>100</v>
       </c>
       <c r="D42">
-        <v>66.207958716284466</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E42">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F42">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G42">
-        <v>2.8568857142857138</v>
+        <v>0.26491422725817698</v>
+      </c>
+      <c r="G42" t="s">
+        <v>18</v>
       </c>
       <c r="H42">
+        <v>0.99999999992750455</v>
+      </c>
+      <c r="I42">
         <v>33.789000000000001</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>99.991</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>66.201999999999998</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>35</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <v>66.201999999999998</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>33.789000000000001</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>2</v>
       </c>
-      <c r="P42">
-        <v>2.5361537842447608</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q42">
+        <v>2.0625941567536841</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B43">
         <v>70</v>
@@ -2602,48 +2869,51 @@
         <v>100</v>
       </c>
       <c r="D43">
+        <v>1.0328250276619559</v>
+      </c>
+      <c r="E43">
+        <v>2.1132402255538891E-4</v>
+      </c>
+      <c r="F43">
+        <v>2.0191531248405958</v>
+      </c>
+      <c r="G43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43">
+        <v>0.99999999989156385</v>
+      </c>
+      <c r="I43">
+        <v>99.665999999999997</v>
+      </c>
+      <c r="J43">
+        <v>100</v>
+      </c>
+      <c r="K43">
         <v>0.33400000000000002</v>
       </c>
-      <c r="E43">
-        <v>1.035214093657288</v>
-      </c>
-      <c r="F43">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G43">
+      <c r="L43">
         <v>10</v>
       </c>
-      <c r="H43">
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="O43">
         <v>99.665999999999997</v>
       </c>
-      <c r="I43">
-        <v>100</v>
-      </c>
-      <c r="J43">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="K43">
-        <v>10</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="N43">
-        <v>99.665999999999997</v>
-      </c>
-      <c r="O43">
+      <c r="P43">
         <v>3</v>
       </c>
-      <c r="P43">
-        <v>1.474579313735402</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q43">
+        <v>1.5282974571974199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B44">
         <v>70</v>
@@ -2652,48 +2922,51 @@
         <v>200</v>
       </c>
       <c r="D44">
+        <v>5.3069273602759067E-3</v>
+      </c>
+      <c r="E44">
+        <v>1.7955562058679719E-2</v>
+      </c>
+      <c r="F44">
+        <v>3.7512652839869709</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44">
+        <v>0.99999672911425386</v>
+      </c>
+      <c r="I44">
+        <v>4.6470000000000002</v>
+      </c>
+      <c r="J44">
+        <v>100</v>
+      </c>
+      <c r="K44">
         <v>95.352999999999994</v>
       </c>
-      <c r="E44">
-        <v>5.4209688095402048E-3</v>
-      </c>
-      <c r="F44">
-        <v>1.8010971763348291E-2</v>
-      </c>
-      <c r="G44">
-        <v>20</v>
-      </c>
-      <c r="H44">
-        <v>4.6470000000000002</v>
-      </c>
-      <c r="I44">
-        <v>100</v>
-      </c>
-      <c r="J44">
-        <v>95.352999999999994</v>
-      </c>
-      <c r="K44">
+      <c r="L44">
         <v>5</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>0</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <v>190.70599999999999</v>
       </c>
-      <c r="N44">
+      <c r="O44">
         <v>9.2940000000000005</v>
       </c>
-      <c r="O44">
+      <c r="P44">
         <v>1</v>
       </c>
-      <c r="P44">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q44">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B45">
         <v>70</v>
@@ -2702,48 +2975,51 @@
         <v>200</v>
       </c>
       <c r="D45">
-        <v>66.208289787529822</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="E45">
-        <v>6.8791637143082077E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="F45">
-        <v>3.644373996879021E-6</v>
-      </c>
-      <c r="G45">
-        <v>2.856871428571429</v>
+        <v>0.26491568061954651</v>
+      </c>
+      <c r="G45" t="s">
+        <v>18</v>
       </c>
       <c r="H45">
+        <v>0.99999999999323608</v>
+      </c>
+      <c r="I45">
         <v>33.788499999999999</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>99.990499999999997</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>66.201999999999998</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>35</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>1.9E-2</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>132.404</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>67.576999999999998</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>2</v>
       </c>
-      <c r="P45">
-        <v>2.5778698971056859</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q45">
+        <v>2.0930784905823319</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B46">
         <v>70</v>
@@ -2752,43 +3028,46 @@
         <v>200</v>
       </c>
       <c r="D46">
+        <v>1.0328250276619559</v>
+      </c>
+      <c r="E46">
+        <v>2.1132402255538891E-4</v>
+      </c>
+      <c r="F46">
+        <v>2.0191734141840452</v>
+      </c>
+      <c r="G46" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46">
+        <v>0.99999999997951927</v>
+      </c>
+      <c r="I46">
+        <v>99.665499999999994</v>
+      </c>
+      <c r="J46">
+        <v>100</v>
+      </c>
+      <c r="K46">
         <v>0.33450000000000002</v>
       </c>
-      <c r="E46">
-        <v>1.035214093657288</v>
-      </c>
-      <c r="F46">
-        <v>2.1037593661425911E-4</v>
-      </c>
-      <c r="G46">
+      <c r="L46">
         <v>10</v>
       </c>
-      <c r="H46">
-        <v>99.665499999999994</v>
-      </c>
-      <c r="I46">
-        <v>100</v>
-      </c>
-      <c r="J46">
-        <v>0.33450000000000002</v>
-      </c>
-      <c r="K46">
-        <v>10</v>
-      </c>
-      <c r="L46">
+      <c r="M46">
         <v>0</v>
       </c>
-      <c r="M46">
+      <c r="N46">
         <v>0.66900000000000004</v>
       </c>
-      <c r="N46">
+      <c r="O46">
         <v>199.33099999999999</v>
       </c>
-      <c r="O46">
+      <c r="P46">
         <v>3</v>
       </c>
-      <c r="P46">
-        <v>1.47457958108827</v>
+      <c r="Q46">
+        <v>1.522104213449615</v>
       </c>
     </row>
   </sheetData>
@@ -2809,72 +3088,72 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>4.1596418884308921</v>
+        <v>3.4596418884308928</v>
       </c>
       <c r="C2">
-        <v>0.78353354258501828</v>
+        <v>0.78353354258501839</v>
       </c>
       <c r="D2">
         <v>15</v>
       </c>
       <c r="E2">
-        <v>96.604643856343415</v>
+        <v>96.443933333333334</v>
       </c>
       <c r="F2">
-        <v>96.443933333333334</v>
+        <v>99.834000000000003</v>
       </c>
       <c r="G2">
-        <v>99.834000000000003</v>
+        <v>3.3900333333333328</v>
       </c>
       <c r="H2">
-        <v>3.3900333333333328</v>
+        <v>1.895228408050647</v>
       </c>
       <c r="I2">
-        <v>19.966799999999999</v>
+        <v>5.3069273602759084E-3</v>
       </c>
       <c r="J2">
-        <v>5.4209688095402074E-3</v>
+        <v>1.7955562058679712E-2</v>
       </c>
       <c r="K2">
-        <v>1.8010971763348281E-2</v>
+        <v>0.99996295117474432</v>
       </c>
       <c r="L2">
         <v>15</v>
@@ -2882,37 +3161,37 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>2.8529475588175388</v>
+        <v>2.3272407789963898</v>
       </c>
       <c r="C3">
-        <v>0.78604338311292332</v>
+        <v>0.79284867905768641</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>75.079744003775104</v>
+        <v>74.909333333333336</v>
       </c>
       <c r="F3">
-        <v>74.909333333333336</v>
+        <v>99.783933333333337</v>
       </c>
       <c r="G3">
-        <v>99.783933333333337</v>
+        <v>24.8748</v>
       </c>
       <c r="H3">
-        <v>24.8748</v>
+        <v>0.19408146868686249</v>
       </c>
       <c r="I3">
-        <v>2.8509695238095238</v>
+        <v>6.7253433350914854E-2</v>
       </c>
       <c r="J3">
-        <v>6.8791637143082091E-2</v>
+        <v>2.884042522964212E-6</v>
       </c>
       <c r="K3">
-        <v>3.6443739968790202E-6</v>
+        <v>0.99999999992777622</v>
       </c>
       <c r="L3">
         <v>15</v>
@@ -2920,40 +3199,257 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>1.30470628208133</v>
+        <v>1.388217137001444</v>
       </c>
       <c r="C4">
-        <v>0.746106633459375</v>
+        <v>0.71703479768019851</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>10.68021920235218</v>
+        <v>10.641866666666671</v>
       </c>
       <c r="F4">
-        <v>10.641866666666671</v>
+        <v>99.866733333333329</v>
       </c>
       <c r="G4">
-        <v>99.866733333333329</v>
+        <v>89.224899999999991</v>
       </c>
       <c r="H4">
-        <v>89.224899999999991</v>
+        <v>1.162172232009961</v>
       </c>
       <c r="I4">
-        <v>9.986673333333334</v>
+        <v>1.0328250276619571</v>
       </c>
       <c r="J4">
-        <v>1.035214093657288</v>
+        <v>2.113240225553888E-4</v>
       </c>
       <c r="K4">
-        <v>2.1037593661425919E-4</v>
+        <v>0.99999999979956244</v>
       </c>
       <c r="L4">
         <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>